<commit_message>
added script for further running exp with pfeature feature and other exploration
</commit_message>
<xml_diff>
--- a/data/text/AVP_IC50_test_res_server.xlsx
+++ b/data/text/AVP_IC50_test_res_server.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/in-divye.singh/Documents/Projects/MIC_predictor/data/text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9829B1B2-2AE2-4840-A739-39CF97DB3FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17CB85E-D92F-694B-80AC-CF4C0CACEEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="248898462" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'248898462'!$A$1:$K$77</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
   <si>
     <t>Fasta ID</t>
   </si>
@@ -516,13 +519,34 @@
     <t>MAPE</t>
   </si>
   <si>
-    <t>Abs Perc Err</t>
+    <t>our_model</t>
+  </si>
+  <si>
+    <t>Abs Perc Err_server</t>
+  </si>
+  <si>
+    <t>Abs Perc Err_model</t>
+  </si>
+  <si>
+    <t>Corr MIC - Err (our)</t>
+  </si>
+  <si>
+    <t>Corr MIC - Err (server)</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Our</t>
+  </si>
+  <si>
+    <t>PCC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1013,11 +1037,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1074,6 +1099,2309 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Server</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'248898462'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IC50_(microM)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'248898462'!$D$2:$D$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>201.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227.93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>261.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>270.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121.77</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>106.22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42.95</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50.41</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.65</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44.22</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.04</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.07</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56.41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.81</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33.81</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.29</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33.909999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21.56</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45.81</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.41</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.83</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28.75</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.25</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16.43</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>52.02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.89</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>27.66</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>32.15</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45.22</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17.52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>55.02</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11.16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.39</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>39.22</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.34</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>28.23</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.66</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>17.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>38.4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14.13</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>38.72</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.17</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>29.44</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>39.83</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28.27</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.7699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>29.31</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>48.26</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>12.87</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.21</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'248898462'!$I$2:$I$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>258.34399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.299000000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.607999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37.128</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.515000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.86</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.7200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.6190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.53100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.46400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.22800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.57</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B796-6145-99B4-23FC85F03DB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1334751360"/>
+        <c:axId val="1404251776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1334751360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Predicted</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404251776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1404251776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Actual</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1334751360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Our model</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'248898462'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IC50_(microM)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'248898462'!$H$2:$H$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.135999999999903</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36.590000000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16.329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.89900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.5000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>19.745000000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>35.4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.00E+00">
+                  <c:v>2.9999999999999899E-5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.36199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.347</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>53.753</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.2999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.13099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'248898462'!$I$2:$I$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>258.34399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.299000000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.607999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37.128</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.515000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.86</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.7200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.6190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.53100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.46400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.22800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.57</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-06C1-6D4D-B6FA-48B6A8C0BF19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1334751360"/>
+        <c:axId val="1404251776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1334751360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Predicted</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404251776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1404251776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Actual</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1334751360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ABB3158-5196-384B-AC28-6EEEF739727F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A228FFE9-CC04-144D-B013-88B41F366EB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1372,22 +3700,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1409,14 +3739,26 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1438,22 +3780,33 @@
       <c r="G2">
         <v>90.01</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
+        <v>62</v>
+      </c>
+      <c r="I2" s="2">
         <v>333</v>
       </c>
-      <c r="I2">
-        <f>100*(ABS(D2-H2)/H2)</f>
+      <c r="J2">
+        <f>100*(ABS(D2-I2)/I2)</f>
         <v>39.471471471471467</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="M2">
-        <f>AVERAGE(I2:I77)</f>
+      <c r="K2">
+        <f>100*(ABS(H2-I2)/I2)</f>
+        <v>81.381381381381374</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(J2:J77)</f>
         <v>6752.890921178755</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <f>CORREL(D2:D76,I2:I76)</f>
+        <v>0.70342330206540138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1475,15 +3828,33 @@
       <c r="G3">
         <v>277.01</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
+        <v>277</v>
+      </c>
+      <c r="I3" s="2">
         <v>294</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I66" si="0">100*(ABS(D3-H3)/H3)</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J66" si="0">100*(ABS(D3-I3)/I3)</f>
         <v>22.472789115646254</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="1">100*(ABS(H3-I3)/I3)</f>
+        <v>5.7823129251700678</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N3">
+        <f>AVERAGE(K2:K77)</f>
+        <v>1710.4256898338665</v>
+      </c>
+      <c r="O3">
+        <f>CORREL(H2:H76,I2:I76)</f>
+        <v>0.43685485794635381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1505,15 +3876,22 @@
       <c r="G4">
         <v>1.44</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2">
         <v>258.34399999999999</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>82.534914687393552</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>92.258384169943952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1535,15 +3913,22 @@
       <c r="G5">
         <v>3.51</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
+        <v>3.5</v>
+      </c>
+      <c r="I5" s="2">
         <v>150</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>74.333333333333329</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>97.666666666666671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1565,15 +3950,29 @@
       <c r="G6">
         <v>5.01</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
         <v>124</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>52.951612903225808</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>95.967741935483872</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="N6">
+        <f>CORREL(I2:I77,K2:K77)</f>
+        <v>-0.10555441633837938</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1595,15 +3994,29 @@
       <c r="G7">
         <v>4.8099999999999996</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
+        <v>4.8</v>
+      </c>
+      <c r="I7" s="2">
         <v>119</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>35.907563025210088</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>95.966386554621849</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N7">
+        <f>CORREL(I2:I77,J2:J77)</f>
+        <v>-9.9586042536231753E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1625,15 +4038,22 @@
       <c r="G8">
         <v>14.8</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>100</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
+        <v>100</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>58.91</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1655,15 +4075,22 @@
       <c r="G9">
         <v>23.47</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
+        <v>23.46</v>
+      </c>
+      <c r="I9" s="2">
         <v>100</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>63.840000000000011</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>76.539999999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1685,15 +4112,22 @@
       <c r="G10">
         <v>90.01</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
+        <v>333</v>
+      </c>
+      <c r="I10" s="2">
         <v>95</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>185.05263157894737</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>250.52631578947367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1715,15 +4149,22 @@
       <c r="G11">
         <v>8.51</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
+        <v>25</v>
+      </c>
+      <c r="I11" s="2">
         <v>88.299000000000007</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>56.194294386119893</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>71.687108574276039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1745,15 +4186,22 @@
       <c r="G12">
         <v>21.01</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
+        <v>21</v>
+      </c>
+      <c r="I12" s="2">
         <v>83</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>46.710843373493972</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>74.698795180722882</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1775,15 +4223,22 @@
       <c r="G13">
         <v>56.01</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
+        <v>34.135999999999903</v>
+      </c>
+      <c r="I13" s="2">
         <v>60.607999999999997</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>65.539202745512142</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>43.677402323125818</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1805,15 +4260,22 @@
       <c r="G14">
         <v>313.01</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I14" s="2">
         <v>50</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>112.44000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>99.977999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1835,15 +4297,22 @@
       <c r="G15">
         <v>32.71</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="I15" s="2">
         <v>50</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>14.099999999999993</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>99.997399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1865,15 +4334,22 @@
       <c r="G16">
         <v>313.01</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
+        <v>1.7</v>
+      </c>
+      <c r="I16" s="2">
         <v>50</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>0.81999999999999318</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>96.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1895,15 +4371,22 @@
       <c r="G17">
         <v>0.36</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
+        <v>0.35</v>
+      </c>
+      <c r="I17" s="2">
         <v>44</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>37.159090909090914</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>99.204545454545453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1925,15 +4408,22 @@
       <c r="G18">
         <v>47.31</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
+        <v>47.3</v>
+      </c>
+      <c r="I18" s="2">
         <v>40.799999999999997</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>8.3823529411764763</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>15.93137254901961</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1955,15 +4445,22 @@
       <c r="G19">
         <v>1.2</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
+        <v>1.19</v>
+      </c>
+      <c r="I19" s="2">
         <v>37.128</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>59.491488903253611</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>96.79487179487181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1985,15 +4482,22 @@
       <c r="G20">
         <v>4.01</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
+        <v>1.2</v>
+      </c>
+      <c r="I20" s="2">
         <v>30</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>87.966666666666669</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>96.000000000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2015,15 +4519,22 @@
       <c r="G21">
         <v>17.5</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21" s="2">
         <v>27</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>59.518518518518512</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>81.481481481481481</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2045,15 +4556,22 @@
       <c r="G22">
         <v>4.3099999999999996</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22">
+        <v>4.3</v>
+      </c>
+      <c r="I22" s="2">
         <v>25</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>82.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2075,15 +4593,22 @@
       <c r="G23">
         <v>7.61</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23">
+        <v>7.6</v>
+      </c>
+      <c r="I23" s="2">
         <v>25</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>125.64</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>69.599999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2105,15 +4630,22 @@
       <c r="G24">
         <v>2.0299999999999998</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24">
+        <v>24</v>
+      </c>
+      <c r="I24" s="2">
         <v>25</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>48.76</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2135,15 +4667,22 @@
       <c r="G25">
         <v>0.04</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I25" s="2">
         <v>25</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>35.240000000000009</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>99.896000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2165,15 +4704,22 @@
       <c r="G26">
         <v>25.01</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26">
         <v>23.8</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="0"/>
         <v>10.462184873949573</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2195,15 +4741,22 @@
       <c r="G27">
         <v>36.6</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27">
+        <v>36.590000000000003</v>
+      </c>
+      <c r="I27" s="2">
         <v>22.16</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="0"/>
         <v>53.023465703971105</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>65.117328519855604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -2225,15 +4778,22 @@
       <c r="G28">
         <v>5.01</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28" s="2">
         <v>21</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="0"/>
         <v>2.6666666666666607</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>76.19047619047619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2255,15 +4815,22 @@
       <c r="G29">
         <v>4.01</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29" s="2">
         <v>17.8</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f t="shared" si="0"/>
         <v>88.089887640449433</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>77.528089887640448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -2285,15 +4852,22 @@
       <c r="G30">
         <v>44.01</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30">
+        <v>12</v>
+      </c>
+      <c r="I30" s="2">
         <v>14.515000000000001</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <f t="shared" si="0"/>
         <v>215.60454702032379</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>17.326903203582507</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2315,15 +4889,22 @@
       <c r="G31">
         <v>220.01</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31">
+        <v>220</v>
+      </c>
+      <c r="I31" s="2">
         <v>14</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <f t="shared" si="0"/>
         <v>25.642857142857139</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>1471.4285714285713</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -2345,15 +4926,22 @@
       <c r="G32">
         <v>6.01</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32">
+        <v>13</v>
+      </c>
+      <c r="I32" s="2">
         <v>12</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <f t="shared" si="0"/>
         <v>6.6666666666666723</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333321</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -2375,15 +4963,22 @@
       <c r="G33">
         <v>2.0099999999999998</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33" s="2">
         <v>12</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <f t="shared" si="0"/>
         <v>1.4166666666666661</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2405,15 +5000,22 @@
       <c r="G34">
         <v>4.01</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34" s="2">
         <v>12</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <f t="shared" si="0"/>
         <v>28.333333333333339</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -2435,15 +5037,22 @@
       <c r="G35">
         <v>18.48</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35">
+        <v>7.6</v>
+      </c>
+      <c r="I35" s="2">
         <v>10.86</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <f t="shared" si="0"/>
         <v>164.7329650092081</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>30.018416206261513</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2465,15 +5074,22 @@
       <c r="G36">
         <v>0.21</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36">
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="2">
         <v>10</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <f t="shared" si="0"/>
         <v>71.499999999999986</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2495,15 +5111,22 @@
       <c r="G37">
         <v>11.01</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="I37" s="2">
         <v>9.7200000000000006</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <f t="shared" si="0"/>
         <v>77.469135802469125</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>68.004115226337419</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -2525,15 +5148,22 @@
       <c r="G38">
         <v>8.01</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38">
+        <v>30</v>
+      </c>
+      <c r="I38" s="2">
         <v>9</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <f t="shared" si="0"/>
         <v>82.555555555555543</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>233.33333333333334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -2555,15 +5185,22 @@
       <c r="G39">
         <v>6.01</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39">
         <v>8</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="2">
+        <v>8</v>
+      </c>
+      <c r="J39">
         <f t="shared" si="0"/>
         <v>550.25</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -2585,15 +5222,22 @@
       <c r="G40">
         <v>12.31</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40">
+        <v>0.02</v>
+      </c>
+      <c r="I40" s="2">
         <v>7.3</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <f t="shared" si="0"/>
         <v>76.575342465753437</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>99.726027397260282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2615,15 +5259,22 @@
       <c r="G41">
         <v>2.11</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41">
         <v>7.1</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="2">
+        <v>7.1</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="0"/>
         <v>289.57746478873247</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2645,15 +5296,22 @@
       <c r="G42">
         <v>1.41</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42">
         <v>7</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="2">
+        <v>7</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="0"/>
         <v>359.28571428571428</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -2675,15 +5333,22 @@
       <c r="G43">
         <v>0.87</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43" s="2">
         <v>7</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <f t="shared" si="0"/>
         <v>546</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>14.285714285714285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2705,15 +5370,22 @@
       <c r="G44">
         <v>5.01</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44">
+        <v>11</v>
+      </c>
+      <c r="I44" s="2">
         <v>7</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <f t="shared" si="0"/>
         <v>150.28571428571428</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>57.142857142857139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -2735,15 +5407,22 @@
       <c r="G45">
         <v>29.01</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45">
         <v>5</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="2">
+        <v>5</v>
+      </c>
+      <c r="J45">
         <f t="shared" si="0"/>
         <v>1000.4000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -2765,15 +5444,22 @@
       <c r="G46">
         <v>0.8</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46">
+        <v>1.7</v>
+      </c>
+      <c r="I46" s="2">
         <v>4.7</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <f t="shared" si="0"/>
         <v>137.44680851063828</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>63.829787234042549</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -2795,15 +5481,22 @@
       <c r="G47">
         <v>2.11</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47">
+        <v>3.5</v>
+      </c>
+      <c r="I47" s="2">
         <v>3.9</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <f t="shared" si="0"/>
         <v>63.84615384615384</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>10.256410256410255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2825,15 +5518,22 @@
       <c r="G48">
         <v>10.52</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48">
         <v>3.69</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="J48">
         <f t="shared" si="0"/>
         <v>962.8726287262873</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>101</v>
       </c>
@@ -2855,15 +5555,22 @@
       <c r="G49">
         <v>1.41</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49">
         <v>3.5</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="J49">
         <f t="shared" si="0"/>
         <v>138.28571428571428</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2885,15 +5592,22 @@
       <c r="G50">
         <v>2.86</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50">
         <v>3</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="2">
+        <v>3</v>
+      </c>
+      <c r="J50">
         <f t="shared" si="0"/>
         <v>841</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -2915,15 +5629,22 @@
       <c r="G51">
         <v>0.91</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="I51" s="2">
         <v>3</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <f t="shared" si="0"/>
         <v>63.666666666666657</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <f t="shared" si="1"/>
+        <v>70.033333333333331</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2945,15 +5666,22 @@
       <c r="G52">
         <v>4.51</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52">
+        <v>4.5</v>
+      </c>
+      <c r="I52" s="2">
         <v>3</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <f t="shared" si="0"/>
         <v>108.66666666666667</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2975,15 +5703,22 @@
       <c r="G53">
         <v>0.09</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="I53" s="2">
         <v>3</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <f t="shared" si="0"/>
         <v>653.33333333333337</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <f t="shared" si="1"/>
+        <v>97.166666666666671</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -3005,15 +5740,22 @@
       <c r="G54">
         <v>19.75</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54">
+        <v>19.745000000000001</v>
+      </c>
+      <c r="I54" s="2">
         <v>2.6190000000000002</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <f t="shared" si="0"/>
         <v>1948.8736158839249</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <f t="shared" si="1"/>
+        <v>653.91370752195485</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -3035,15 +5777,22 @@
       <c r="G55">
         <v>7.61</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55">
+        <v>7.6</v>
+      </c>
+      <c r="I55" s="2">
         <v>2.1</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <f t="shared" si="0"/>
         <v>86.19047619047619</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <f t="shared" si="1"/>
+        <v>261.90476190476193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -3065,15 +5814,22 @@
       <c r="G56">
         <v>0.2</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56">
+        <v>0.19</v>
+      </c>
+      <c r="I56" s="2">
         <v>1.55</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <f t="shared" si="0"/>
         <v>25.161290322580637</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <f t="shared" si="1"/>
+        <v>87.741935483870975</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -3095,15 +5851,22 @@
       <c r="G57">
         <v>9.01</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57">
+        <v>9</v>
+      </c>
+      <c r="I57" s="2">
         <v>1.52</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <f t="shared" si="0"/>
         <v>1019.0789473684213</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <f t="shared" si="1"/>
+        <v>492.1052631578948</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -3125,15 +5888,22 @@
       <c r="G58">
         <v>1.21</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58">
+        <v>35.4</v>
+      </c>
+      <c r="I58" s="2">
         <v>1.4</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <f t="shared" si="0"/>
         <v>2642.8571428571431</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <f t="shared" si="1"/>
+        <v>2428.5714285714289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -3155,15 +5925,22 @@
       <c r="G59">
         <v>6.83</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I59" s="2">
         <v>1.19</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <f t="shared" si="0"/>
         <v>310.0840336134454</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <f t="shared" si="1"/>
+        <v>89.915966386554615</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -3185,15 +5962,22 @@
       <c r="G60">
         <v>0.19</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60">
+        <v>0.18</v>
+      </c>
+      <c r="I60" s="2">
         <v>0.84</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <f t="shared" si="0"/>
         <v>1582.1428571428573</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <f t="shared" si="1"/>
+        <v>78.571428571428569</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -3215,15 +5999,22 @@
       <c r="G61">
         <v>1.21</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61">
         <v>0.82</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="J61">
         <f t="shared" si="0"/>
         <v>26.829268292682922</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>127</v>
       </c>
@@ -3245,15 +6036,22 @@
       <c r="G62">
         <v>2.86</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62">
+        <v>3</v>
+      </c>
+      <c r="I62" s="2">
         <v>0.75</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <f t="shared" si="0"/>
         <v>5062.6666666666661</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>129</v>
       </c>
@@ -3275,15 +6073,22 @@
       <c r="G63">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I63" s="2">
         <v>0.73</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <f t="shared" si="0"/>
         <v>334.24657534246575</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <f t="shared" si="1"/>
+        <v>61.643835616438345</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -3305,15 +6110,22 @@
       <c r="G64">
         <v>0.23</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64">
+        <v>0.22</v>
+      </c>
+      <c r="I64" s="2">
         <v>0.7</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <f t="shared" si="0"/>
         <v>4105.7142857142862</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <f t="shared" si="1"/>
+        <v>68.571428571428569</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -3335,15 +6147,22 @@
       <c r="G65">
         <v>1.49</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="4">
+        <v>2.9999999999999899E-5</v>
+      </c>
+      <c r="I65" s="2">
         <v>0.63800000000000001</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <f t="shared" si="0"/>
         <v>6142.94670846395</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <f t="shared" si="1"/>
+        <v>99.995297805642636</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -3365,15 +6184,22 @@
       <c r="G66">
         <v>0.35</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66">
+        <v>7</v>
+      </c>
+      <c r="I66" s="2">
         <v>0.53100000000000003</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <f t="shared" si="0"/>
         <v>5223.9171374764592</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <f t="shared" si="1"/>
+        <v>1218.2674199623352</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>137</v>
       </c>
@@ -3395,15 +6221,22 @@
       <c r="G67">
         <v>0.8</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67">
         <v>0.5</v>
       </c>
-      <c r="I67">
-        <f t="shared" ref="I67:I77" si="1">100*(ABS(D67-H67)/H67)</f>
+      <c r="I67" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J67">
+        <f t="shared" ref="J67:J77" si="2">100*(ABS(D67-I67)/I67)</f>
         <v>853.99999999999989</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <f t="shared" ref="K67:K77" si="3">100*(ABS(H67-I67)/I67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -3425,15 +6258,22 @@
       <c r="G68">
         <v>7.01</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="I68" s="2">
         <v>0.48799999999999999</v>
       </c>
-      <c r="I68">
-        <f t="shared" si="1"/>
+      <c r="J68">
+        <f t="shared" si="2"/>
         <v>5906.1475409836066</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <f t="shared" si="3"/>
+        <v>25.819672131147541</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -3455,15 +6295,22 @@
       <c r="G69">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69">
+        <v>1.347</v>
+      </c>
+      <c r="I69" s="2">
         <v>0.46400000000000002</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="1"/>
+      <c r="J69">
+        <f t="shared" si="2"/>
         <v>255.60344827586206</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <f t="shared" si="3"/>
+        <v>190.30172413793102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -3485,15 +6332,22 @@
       <c r="G70">
         <v>0.13</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I70" s="2">
         <v>0.22800000000000001</v>
       </c>
-      <c r="I70">
-        <f t="shared" si="1"/>
+      <c r="J70">
+        <f t="shared" si="2"/>
         <v>21066.666666666664</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <f t="shared" si="3"/>
+        <v>90.789473684210535</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -3515,15 +6369,22 @@
       <c r="G71">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71">
+        <v>53.753</v>
+      </c>
+      <c r="I71" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="I71">
-        <f t="shared" si="1"/>
+      <c r="J71">
+        <f t="shared" si="2"/>
         <v>13591.489361702128</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <f t="shared" si="3"/>
+        <v>57084.042553191488</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -3545,15 +6406,22 @@
       <c r="G72">
         <v>0.04</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I72" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I72">
-        <f t="shared" si="1"/>
+      <c r="J72">
+        <f t="shared" si="2"/>
         <v>6878.260869565217</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <f t="shared" si="3"/>
+        <v>6.5217391304347876</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -3575,15 +6443,22 @@
       <c r="G73">
         <v>0.01</v>
       </c>
-      <c r="H73" s="2">
+      <c r="H73">
+        <v>1.13099999999999E-2</v>
+      </c>
+      <c r="I73" s="2">
         <v>7.57</v>
       </c>
-      <c r="I73">
-        <f t="shared" si="1"/>
+      <c r="J73">
+        <f t="shared" si="2"/>
         <v>56.406869220607668</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <f t="shared" si="3"/>
+        <v>99.850594451783365</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>151</v>
       </c>
@@ -3605,15 +6480,22 @@
       <c r="G74">
         <v>0.03</v>
       </c>
-      <c r="H74" s="2">
+      <c r="H74">
+        <v>3</v>
+      </c>
+      <c r="I74" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I74">
-        <f t="shared" si="1"/>
+      <c r="J74">
+        <f t="shared" si="2"/>
         <v>120150</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <f t="shared" si="3"/>
+        <v>37400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -3635,15 +6517,22 @@
       <c r="G75">
         <v>0.01</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I75" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="I75">
-        <f t="shared" si="1"/>
+      <c r="J75">
+        <f t="shared" si="2"/>
         <v>19233.333333333332</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -3665,15 +6554,22 @@
       <c r="G76">
         <v>0.67</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="I76" s="2">
         <v>2E-3</v>
       </c>
-      <c r="I76">
-        <f t="shared" si="1"/>
+      <c r="J76">
+        <f t="shared" si="2"/>
         <v>288400</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K76">
+        <f t="shared" si="3"/>
+        <v>24050</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -3683,15 +6579,24 @@
       <c r="C77">
         <v>0</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I77" s="2">
         <v>2E-3</v>
       </c>
-      <c r="I77">
-        <f t="shared" si="1"/>
+      <c r="J77">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
+      <c r="K77">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K77" xr:uid="{CCD9D8DA-C564-9F40-B6D3-6A27D52EA6C1}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>